<commit_message>
Made changes to the sprint
</commit_message>
<xml_diff>
--- a/Scrum/SPRINT BACKLOG/SprintBacklog2.xlsx
+++ b/Scrum/SPRINT BACKLOG/SprintBacklog2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itumeleng Malematja\Desktop\COMPUTER SCIENCE\COS301\FINAL PROJECT\COEUS\ADMIN\SPRINT BACKLOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itumeleng Malematja\Desktop\COMPUTER SCIENCE\COS301\FINAL PROJECT\COEUS\GeospatialDataProcessorVisualiser_documentation\Scrum\SPRINT BACKLOG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,45 +498,9 @@
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,9 +525,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,12 +533,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -620,6 +575,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,11 +887,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1250605888"/>
-        <c:axId val="1250606976"/>
+        <c:axId val="624166592"/>
+        <c:axId val="551475392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1250605888"/>
+        <c:axId val="624166592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1250606976"/>
+        <c:crossAx val="551475392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -941,7 +941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1250606976"/>
+        <c:axId val="551475392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1250605888"/>
+        <c:crossAx val="624166592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1633,16 +1633,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2045,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,679 +2057,679 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="6"/>
-      <c r="T2" s="7" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="44"/>
+      <c r="T2" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="14"/>
+      <c r="T3" s="46"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="5">
         <v>6</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="20"/>
-      <c r="T4" s="21">
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="8"/>
+      <c r="T4" s="9">
         <f>SUM(E4:R4)</f>
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="11">
         <v>20</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24">
+      <c r="E5" s="6"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12">
         <v>3</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="12">
         <v>5</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24">
+      <c r="J5" s="12"/>
+      <c r="K5" s="12">
         <v>2</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="12">
         <v>2</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="12">
         <v>2</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="12">
         <v>2</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="12">
         <v>2</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="12">
         <v>2</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="12">
         <v>2</v>
       </c>
-      <c r="R5" s="20">
+      <c r="R5" s="8">
         <v>2</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="9">
         <f>SUM(E5:R5)</f>
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="11">
         <v>5</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24">
+      <c r="E6" s="6"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12">
         <v>2</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="12">
         <v>2</v>
       </c>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24">
+      <c r="M6" s="12"/>
+      <c r="N6" s="12">
         <v>1</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="12">
         <v>1</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="20"/>
-      <c r="T6" s="21">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="8"/>
+      <c r="T6" s="9">
         <f t="shared" ref="T6:T17" si="0">SUM(E6:R6)</f>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="11">
         <v>20</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24">
+      <c r="E7" s="6"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12">
         <v>5</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="12">
         <v>3</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="12">
         <v>3</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="12">
         <v>4</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="12">
         <v>2</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="8">
         <v>1</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="11">
         <v>1</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24">
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12">
         <v>2</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="20"/>
-      <c r="T8" s="21">
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="8"/>
+      <c r="T8" s="9">
         <f>SUM(E8:R8)</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="20"/>
-      <c r="T9" s="21">
+      <c r="B9" s="47"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="8"/>
+      <c r="T9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="20"/>
-      <c r="T10" s="21">
+      <c r="B10" s="47"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="8"/>
+      <c r="T10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="14">
         <v>2</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="28"/>
-      <c r="T11" s="29">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="15"/>
+      <c r="T11" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="6">
         <v>1</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="12">
         <v>5</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="12">
         <v>4</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="12">
         <v>3</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="20"/>
-      <c r="T12" s="21">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="8"/>
+      <c r="T12" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="11">
         <v>4</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24">
+      <c r="E13" s="6"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12">
         <v>3</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="12">
         <v>2</v>
       </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="20"/>
-      <c r="T13" s="21">
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="8"/>
+      <c r="T13" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="11">
         <v>8</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24">
+      <c r="E14" s="6"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12">
         <v>1</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="12">
         <v>3</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="12">
         <v>4</v>
       </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="20"/>
-      <c r="T14" s="21">
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="8"/>
+      <c r="T14" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="11">
         <v>48</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24">
+      <c r="E15" s="6"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12">
         <v>2</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="12">
         <v>1</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24">
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12">
         <v>8</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="12">
         <v>9</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15" s="12">
         <v>8</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="12">
         <v>6</v>
       </c>
-      <c r="P15" s="24">
+      <c r="P15" s="12">
         <v>8</v>
       </c>
-      <c r="Q15" s="24">
+      <c r="Q15" s="12">
         <v>7</v>
       </c>
-      <c r="R15" s="20">
+      <c r="R15" s="8">
         <v>6</v>
       </c>
-      <c r="T15" s="21">
+      <c r="T15" s="9">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="20"/>
-      <c r="T16" s="21">
+      <c r="B16" s="34"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="8"/>
+      <c r="T16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="36"/>
-      <c r="T17" s="37">
+      <c r="B17" s="35"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="21"/>
+      <c r="T17" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="24">
         <f>SUM(D4:D17)</f>
         <v>124</v>
       </c>
-      <c r="E19" s="40">
-        <f>D19-SUM(E4:E17)</f>
+      <c r="E19" s="25">
+        <f t="shared" ref="E19:R19" si="1">D19-SUM(E4:E17)</f>
         <v>118</v>
       </c>
-      <c r="F19" s="41">
-        <f>E19-SUM(F4:F17)</f>
+      <c r="F19" s="26">
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="G19" s="41">
-        <f>F19-SUM(G4:G17)</f>
+      <c r="G19" s="26">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="H19" s="41">
-        <f>G19-SUM(H4:H17)</f>
+      <c r="H19" s="26">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="I19" s="41">
-        <f>H19-SUM(I4:I17)</f>
+      <c r="I19" s="26">
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="J19" s="41">
-        <f>I19-SUM(J4:J17)</f>
+      <c r="J19" s="26">
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="K19" s="41">
-        <f>J19-SUM(K4:K17)</f>
+      <c r="K19" s="26">
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="L19" s="41">
-        <f>K19-SUM(L4:L17)</f>
+      <c r="L19" s="26">
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="M19" s="41">
-        <f>L19-SUM(M4:M17)</f>
+      <c r="M19" s="26">
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="N19" s="41">
-        <f>M19-SUM(N4:N17)</f>
+      <c r="N19" s="26">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="O19" s="41">
-        <f>N19-SUM(O4:O17)</f>
+      <c r="O19" s="26">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="P19" s="41">
-        <f>O19-SUM(P4:P17)</f>
+      <c r="P19" s="26">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Q19" s="41">
-        <f>P19-SUM(Q4:Q17)</f>
+      <c r="Q19" s="26">
+        <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="R19" s="42">
-        <f>Q19-SUM(R4:R17)</f>
+      <c r="R19" s="27">
+        <f t="shared" si="1"/>
         <v>-17</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="29">
         <f>SUM(D4:D17)</f>
         <v>124</v>
       </c>
-      <c r="E20" s="45">
-        <f>D20-($D$20/14)</f>
+      <c r="E20" s="30">
+        <f t="shared" ref="E20:R20" si="2">D20-($D$20/14)</f>
         <v>115.14285714285714</v>
       </c>
-      <c r="F20" s="46">
-        <f>E20-($D$20/14)</f>
+      <c r="F20" s="31">
+        <f t="shared" si="2"/>
         <v>106.28571428571428</v>
       </c>
-      <c r="G20" s="46">
-        <f>F20-($D$20/14)</f>
+      <c r="G20" s="31">
+        <f t="shared" si="2"/>
         <v>97.428571428571416</v>
       </c>
-      <c r="H20" s="46">
-        <f>G20-($D$20/14)</f>
+      <c r="H20" s="31">
+        <f t="shared" si="2"/>
         <v>88.571428571428555</v>
       </c>
-      <c r="I20" s="46">
-        <f>H20-($D$20/14)</f>
+      <c r="I20" s="31">
+        <f t="shared" si="2"/>
         <v>79.714285714285694</v>
       </c>
-      <c r="J20" s="46">
-        <f>I20-($D$20/14)</f>
+      <c r="J20" s="31">
+        <f t="shared" si="2"/>
         <v>70.857142857142833</v>
       </c>
-      <c r="K20" s="46">
-        <f>J20-($D$20/14)</f>
+      <c r="K20" s="31">
+        <f t="shared" si="2"/>
         <v>61.999999999999972</v>
       </c>
-      <c r="L20" s="46">
-        <f>K20-($D$20/14)</f>
+      <c r="L20" s="31">
+        <f t="shared" si="2"/>
         <v>53.14285714285711</v>
       </c>
-      <c r="M20" s="46">
-        <f>L20-($D$20/14)</f>
+      <c r="M20" s="31">
+        <f t="shared" si="2"/>
         <v>44.285714285714249</v>
       </c>
-      <c r="N20" s="46">
-        <f>M20-($D$20/14)</f>
+      <c r="N20" s="31">
+        <f t="shared" si="2"/>
         <v>35.428571428571388</v>
       </c>
-      <c r="O20" s="46">
-        <f>N20-($D$20/14)</f>
+      <c r="O20" s="31">
+        <f t="shared" si="2"/>
         <v>26.57142857142853</v>
       </c>
-      <c r="P20" s="46">
-        <f>O20-($D$20/14)</f>
+      <c r="P20" s="31">
+        <f t="shared" si="2"/>
         <v>17.714285714285673</v>
       </c>
-      <c r="Q20" s="46">
-        <f>P20-($D$20/14)</f>
+      <c r="Q20" s="31">
+        <f t="shared" si="2"/>
         <v>8.857142857142815</v>
       </c>
-      <c r="R20" s="47">
-        <f>Q20-($D$20/14)</f>
+      <c r="R20" s="32">
+        <f t="shared" si="2"/>
         <v>-4.2632564145606011E-14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="B4:B10"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:R2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="B4:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>